<commit_message>
Removed some not needed components
</commit_message>
<xml_diff>
--- a/m50,m40,m60 Pnp/Rev 1.0/BOM-speeduino v0.4.3 compatible PCB for m40 rev1.0.xlsx
+++ b/m50,m40,m60 Pnp/Rev 1.0/BOM-speeduino v0.4.3 compatible PCB for m40 rev1.0.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemppain\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C63DFFDF-CC7F-4938-90BC-4C053E45C5F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2B80B0-26C4-4725-8859-92A068EB0BD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16515" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29520" yWindow="1455" windowWidth="25575" windowHeight="14235" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1184,9 +1179,6 @@
     <t>Q1,Q3,Q7,Q8</t>
   </si>
   <si>
-    <t>R11,R14,R37,R48,R49,R56</t>
-  </si>
-  <si>
     <t>R1,R3,R28,R61</t>
   </si>
   <si>
@@ -1239,7 +1231,7 @@
         <color rgb="FF000000"/>
         <rFont val="Liberation Sans"/>
       </rPr>
-      <t>,R50,R51,R58,</t>
+      <t>,R50,R51,</t>
     </r>
     <r>
       <rPr>
@@ -1265,6 +1257,9 @@
       </rPr>
       <t>R64</t>
     </r>
+  </si>
+  <si>
+    <t>R11,R14,R37,R48,R49</t>
   </si>
 </sst>
 </file>
@@ -2056,8 +2051,8 @@
   </sheetPr>
   <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2588,7 +2583,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>192</v>
@@ -2667,7 +2662,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>113</v>
@@ -3018,7 +3013,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>109</v>
@@ -4096,14 +4091,14 @@
     <row r="30" spans="1:24" ht="16.5" thickBot="1">
       <c r="A30" s="18">
         <f>LEN(C30)-LEN(SUBSTITUTE(C30,",",""))+1</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="18">
         <f t="shared" si="36"/>
         <v>13</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>195</v>
@@ -4142,16 +4137,16 @@
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="37"/>
-        <v>0.65999999999999992</v>
+        <v>0.6</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="6"/>
-        <v>1.21</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S30" s="4"/>
       <c r="T30" s="4" t="str">
         <f t="shared" si="24"/>
-        <v>11,1.00KXBK-ND</v>
+        <v>10,1.00KXBK-ND</v>
       </c>
       <c r="U30" s="4" t="str">
         <f t="shared" si="25"/>
@@ -4159,15 +4154,15 @@
       </c>
       <c r="V30" t="str">
         <f t="shared" ref="V30:V36" si="40">"Resistor - " &amp; A30&amp;"x "&amp;E30</f>
-        <v>Resistor - 11x 1k</v>
+        <v>Resistor - 10x 1k</v>
       </c>
       <c r="W30" t="str">
         <f t="shared" si="38"/>
-        <v>603-MFR-25FBF52-1K|11</v>
+        <v>603-MFR-25FBF52-1K|10</v>
       </c>
       <c r="X30" t="str">
         <f t="shared" si="39"/>
-        <v>MFR-25FBF52-1K 11</v>
+        <v>MFR-25FBF52-1K 10</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="16.5" thickBot="1">
@@ -4334,7 +4329,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>197</v>
@@ -4484,14 +4479,14 @@
     <row r="35" spans="1:24" ht="16.5" thickBot="1">
       <c r="A35" s="18">
         <f t="shared" ref="A35" si="41">LEN(C35)-LEN(SUBSTITUTE(C35,",",""))+1</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" s="18">
         <f>LEN(D35)-LEN(SUBSTITUTE(D35,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>112</v>
@@ -4530,16 +4525,16 @@
       </c>
       <c r="Q35" s="6">
         <f t="shared" si="37"/>
-        <v>0.60000000000000009</v>
+        <v>0.5</v>
       </c>
       <c r="R35" s="6">
         <f t="shared" si="6"/>
-        <v>0.60000000000000009</v>
+        <v>0.5</v>
       </c>
       <c r="S35" s="4"/>
       <c r="T35" s="4" t="str">
         <f t="shared" si="24"/>
-        <v>6,100KXBK-ND</v>
+        <v>5,100KXBK-ND</v>
       </c>
       <c r="U35" s="4" t="str">
         <f t="shared" si="25"/>
@@ -4547,15 +4542,15 @@
       </c>
       <c r="V35" t="str">
         <f t="shared" si="40"/>
-        <v>Resistor - 6x 100k</v>
+        <v>Resistor - 5x 100k</v>
       </c>
       <c r="W35" t="str">
         <f t="shared" si="38"/>
-        <v>603-FMF-25FTF52100K|6</v>
+        <v>603-FMF-25FTF52100K|5</v>
       </c>
       <c r="X35" t="str">
         <f t="shared" si="39"/>
-        <v>MFR-25FBF52-100K 6</v>
+        <v>MFR-25FBF52-100K 5</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="16.5" thickBot="1">
@@ -4568,7 +4563,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>110</v>
@@ -5475,11 +5470,11 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="11">
         <f>SUM(Q3:Q49)</f>
-        <v>74.170000000000016</v>
+        <v>74.010000000000005</v>
       </c>
       <c r="R50" s="11">
         <f>SUM(R3:R49)</f>
-        <v>91.920000000000016</v>
+        <v>91.710000000000022</v>
       </c>
       <c r="S50" s="10" t="s">
         <v>69</v>

</xml_diff>